<commit_message>
Se agrega carpeta de User Story y se añaden algunos DTO y algunos Repository
</commit_message>
<xml_diff>
--- a/BASE DE DATOS/Tablas Permisos y Horas extras.xlsx
+++ b/BASE DE DATOS/Tablas Permisos y Horas extras.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="812" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="812" firstSheet="4" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Empleado" sheetId="1" r:id="rId1"/>
@@ -17,13 +17,15 @@
     <sheet name="Permiso" sheetId="7" r:id="rId8"/>
     <sheet name="CategoriaPermisos" sheetId="8" r:id="rId9"/>
     <sheet name="Departamento" sheetId="9" r:id="rId10"/>
+    <sheet name="TiempoExtra" sheetId="12" r:id="rId11"/>
+    <sheet name="Ausencias" sheetId="13" r:id="rId12"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="34">
   <si>
     <t>Atributos</t>
   </si>
@@ -107,6 +109,24 @@
   </si>
   <si>
     <t>Nombre nivel escolaridad</t>
+  </si>
+  <si>
+    <t>Duracion horas</t>
+  </si>
+  <si>
+    <t>Liquidado</t>
+  </si>
+  <si>
+    <t>Hora inicio ausencia</t>
+  </si>
+  <si>
+    <t>Hora fin ausencia</t>
+  </si>
+  <si>
+    <t>Motivo</t>
+  </si>
+  <si>
+    <t>Fecha liquidación</t>
   </si>
 </sst>
 </file>
@@ -550,12 +570,138 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Se agrega carpeta de inicio de proyecto en REACT para frontend
</commit_message>
<xml_diff>
--- a/BASE DE DATOS/Tablas Permisos y Horas extras.xlsx
+++ b/BASE DE DATOS/Tablas Permisos y Horas extras.xlsx
@@ -4,28 +4,28 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="812" firstSheet="4" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="812" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Empleado" sheetId="1" r:id="rId1"/>
     <sheet name="TipoDocIdentidad" sheetId="10" r:id="rId2"/>
     <sheet name="Sexo" sheetId="3" r:id="rId3"/>
-    <sheet name="NivelEscolaridad" sheetId="2" r:id="rId4"/>
-    <sheet name="Rol" sheetId="4" r:id="rId5"/>
-    <sheet name="Turno" sheetId="5" r:id="rId6"/>
-    <sheet name="MarcacionesLlegadas" sheetId="6" r:id="rId7"/>
-    <sheet name="Permiso" sheetId="7" r:id="rId8"/>
-    <sheet name="CategoriaPermisos" sheetId="8" r:id="rId9"/>
-    <sheet name="Departamento" sheetId="9" r:id="rId10"/>
-    <sheet name="TiempoExtra" sheetId="12" r:id="rId11"/>
-    <sheet name="Ausencias" sheetId="13" r:id="rId12"/>
+    <sheet name="Departamento" sheetId="9" r:id="rId4"/>
+    <sheet name="NivelEscolaridad" sheetId="2" r:id="rId5"/>
+    <sheet name="Rol" sheetId="4" r:id="rId6"/>
+    <sheet name="Turno" sheetId="5" r:id="rId7"/>
+    <sheet name="MarcacionesLlegadas" sheetId="6" r:id="rId8"/>
+    <sheet name="Ausencias" sheetId="13" r:id="rId9"/>
+    <sheet name="Permiso" sheetId="7" r:id="rId10"/>
+    <sheet name="CategoriaPermisos" sheetId="8" r:id="rId11"/>
+    <sheet name="TiempoExtra" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="32">
   <si>
     <t>Atributos</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Id</t>
   </si>
   <si>
-    <t>Dia</t>
-  </si>
-  <si>
     <t>Fecha</t>
   </si>
   <si>
@@ -81,12 +78,6 @@
     <t>Hora marcacion 2</t>
   </si>
   <si>
-    <t>Hora marcacion 3</t>
-  </si>
-  <si>
-    <t>Hora marcacion 4</t>
-  </si>
-  <si>
     <t>Fecha inicio</t>
   </si>
   <si>
@@ -127,6 +118,9 @@
   </si>
   <si>
     <t>Fecha liquidación</t>
+  </si>
+  <si>
+    <t>Solo el personal debe timbrarse 2 veces, al inicio y al final de su jornada, en medio de la jornada solo se manejará con permiso aprobado previa validación del vigilante</t>
   </si>
 </sst>
 </file>
@@ -542,15 +536,13 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -562,7 +554,32 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -571,6 +588,41 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A9"/>
   <sheetViews>
@@ -595,7 +647,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
@@ -610,34 +662,276 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -658,349 +952,37 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.42578125" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>